<commit_message>
Atualiza planilha Base de levantamento
Atualização de planilha base
</commit_message>
<xml_diff>
--- a/data/Base de levantamento Sphenophorus.xlsx
+++ b/data/Base de levantamento Sphenophorus.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://breferecombr-my.sharepoint.com/personal/fernando_brefere_com_br/Documents/01_P.A.R.A/01.Projetos/projeto_sphenophorus/dados/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://breferecombr-my.sharepoint.com/personal/fernando_brefere_com_br/Documents/01_P.A.R.A/01.Projetos/projeto_sphenophorus/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="49" documentId="8_{D20646F8-C54A-4EE1-997D-BABB7AF84F48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{50976821-40BE-425C-9AC6-D21B2DB3AAF5}"/>
+  <xr:revisionPtr revIDLastSave="75" documentId="8_{D20646F8-C54A-4EE1-997D-BABB7AF84F48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E0A52029-53EA-4176-B6C1-1C6D6EC7169D}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="11475" xr2:uid="{D8EDB14A-D587-475B-A286-93234BB649C9}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="532" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="530" uniqueCount="67">
   <si>
     <t>Indice de aplicação:</t>
   </si>
@@ -191,36 +191,6 @@
     <t>Testemunha</t>
   </si>
   <si>
-    <t>teste de foto 1</t>
-  </si>
-  <si>
-    <t>teste foto 2</t>
-  </si>
-  <si>
-    <t>teste foto 3</t>
-  </si>
-  <si>
-    <t>C:\Users\fatbr\OneDrive - brefere.com.br\01_P.A.R.A\01.Projetos\projeto_sphenophorus\fotos_sphenophorus\Foto1.jpeg</t>
-  </si>
-  <si>
-    <t>C:\Users\fatbr\OneDrive - brefere.com.br\01_P.A.R.A\01.Projetos\projeto_sphenophorus\fotos_sphenophorus\Foto2.jpg</t>
-  </si>
-  <si>
-    <t>C:\Users\fatbr\OneDrive - brefere.com.br\01_P.A.R.A\01.Projetos\projeto_sphenophorus\fotos_sphenophorus\Foto3.jpg</t>
-  </si>
-  <si>
-    <t>C:\Users\fatbr\OneDrive - brefere.com.br\01_P.A.R.A\01.Projetos\projeto_sphenophorus\fotos_sphenophorus\Foto4.jpg</t>
-  </si>
-  <si>
-    <t>teste foto 4</t>
-  </si>
-  <si>
-    <t>Foto1.jpeg</t>
-  </si>
-  <si>
-    <t>teste arquivo local</t>
-  </si>
-  <si>
     <t>Seu Jose do Canto</t>
   </si>
   <si>
@@ -233,16 +203,40 @@
     <t>RB867515</t>
   </si>
   <si>
-    <t>C:\Users\fatbr\OneDrive - brefere.com.br\01_P.A.R.A\01.Projetos\projeto_sphenophorus\fotos_sphenophorus\Foto5.jpg</t>
+    <t>https://github.com/fatbrefere/projeto_sphenophorus/blob/main/fotos_sphenophorus/Foto1.jpeg</t>
   </si>
   <si>
-    <t>teste de foto 5</t>
+    <t>https://github.com/fatbrefere/projeto_sphenophorus/blob/main/fotos_sphenophorus/Foto2.jpg</t>
   </si>
   <si>
-    <t>Teste foto google drive</t>
+    <t>https://github.com/fatbrefere/projeto_sphenophorus/blob/main/fotos_sphenophorus/Foto3.jpg</t>
   </si>
   <si>
-    <t>https://drive.google.com/uc?export=download&amp;id=1p9dNRLHpB2svligCOEO9WZ-7W91HRuHq</t>
+    <t>https://github.com/fatbrefere/projeto_sphenophorus/blob/main/fotos_sphenophorus/Foto4.jpg</t>
+  </si>
+  <si>
+    <t>https://github.com/fatbrefere/projeto_sphenophorus/blob/main/fotos_sphenophorus/Foto5.jpg</t>
+  </si>
+  <si>
+    <t>https://github.com/fatbrefere/projeto_sphenophorus/blob/main/fotos_sphenophorus/Foto6.jpg</t>
+  </si>
+  <si>
+    <t>Foto 1</t>
+  </si>
+  <si>
+    <t>Foto 2</t>
+  </si>
+  <si>
+    <t>Foto 3</t>
+  </si>
+  <si>
+    <t>Foto 4</t>
+  </si>
+  <si>
+    <t>Foto 5</t>
+  </si>
+  <si>
+    <t>Foto 6</t>
   </si>
 </sst>
 </file>
@@ -1522,8 +1516,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7FB08C5-DA3B-4BF7-B0CE-50F695BC8261}">
   <dimension ref="A1:AK62"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="AD28" workbookViewId="0">
-      <selection activeCell="AF39" sqref="AF39"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="AF1" workbookViewId="0">
+      <selection activeCell="AF9" sqref="AF9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1762,23 +1756,15 @@
         <v>1</v>
       </c>
       <c r="AF3" s="8" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="AG3" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="AH3" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="AI3" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="AJ3" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="AK3" s="4" t="s">
-        <v>53</v>
-      </c>
+        <v>61</v>
+      </c>
+      <c r="AH3" s="8"/>
+      <c r="AI3" s="4"/>
+      <c r="AJ3" s="8"/>
+      <c r="AK3" s="4"/>
     </row>
     <row r="4" spans="1:37" x14ac:dyDescent="0.45">
       <c r="A4" s="4"/>
@@ -1859,10 +1845,10 @@
         <v>2</v>
       </c>
       <c r="AF4" s="8" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="AG4" s="4" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="AH4" s="4"/>
       <c r="AI4" s="4"/>
@@ -1947,8 +1933,12 @@
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="AF5" s="4"/>
-      <c r="AG5" s="4"/>
+      <c r="AF5" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="AG5" s="4" t="s">
+        <v>63</v>
+      </c>
       <c r="AH5" s="4"/>
       <c r="AI5" s="4"/>
       <c r="AJ5" s="4"/>
@@ -2032,8 +2022,12 @@
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="AF6" s="4"/>
-      <c r="AG6" s="4"/>
+      <c r="AF6" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="AG6" s="4" t="s">
+        <v>64</v>
+      </c>
       <c r="AH6" s="4"/>
       <c r="AI6" s="4"/>
       <c r="AJ6" s="4"/>
@@ -2118,10 +2112,10 @@
         <v>2</v>
       </c>
       <c r="AF7" s="4" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="AG7" s="4" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c r="AH7" s="8"/>
       <c r="AI7" s="4"/>
@@ -2206,8 +2200,12 @@
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="AF8" s="4"/>
-      <c r="AG8" s="4"/>
+      <c r="AF8" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="AG8" s="4" t="s">
+        <v>66</v>
+      </c>
       <c r="AH8" s="4"/>
       <c r="AI8" s="4"/>
       <c r="AJ8" s="4"/>
@@ -4261,13 +4259,13 @@
     <row r="33" spans="1:37" x14ac:dyDescent="0.45">
       <c r="A33" s="4"/>
       <c r="B33" s="4" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="D33" s="4" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="E33" s="4">
         <v>1</v>
@@ -4276,7 +4274,7 @@
         <v>1</v>
       </c>
       <c r="G33" s="4" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="H33" s="4">
         <v>4</v>
@@ -4334,12 +4332,8 @@
       <c r="AE33" s="4">
         <v>1</v>
       </c>
-      <c r="AF33" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="AG33" s="4" t="s">
-        <v>66</v>
-      </c>
+      <c r="AF33" s="4"/>
+      <c r="AG33" s="4"/>
       <c r="AH33" s="4"/>
       <c r="AI33" s="4"/>
       <c r="AJ33" s="4"/>
@@ -4348,13 +4342,13 @@
     <row r="34" spans="1:37" x14ac:dyDescent="0.45">
       <c r="A34" s="4"/>
       <c r="B34" s="4" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="D34" s="4" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="E34" s="4">
         <v>1</v>
@@ -4363,7 +4357,7 @@
         <v>1</v>
       </c>
       <c r="G34" s="4" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="H34" s="4">
         <v>4</v>
@@ -4421,12 +4415,8 @@
       <c r="AE34" s="4">
         <v>2</v>
       </c>
-      <c r="AF34" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="AG34" s="4" t="s">
-        <v>67</v>
-      </c>
+      <c r="AF34" s="8"/>
+      <c r="AG34" s="4"/>
       <c r="AH34" s="4"/>
       <c r="AI34" s="4"/>
       <c r="AJ34" s="4"/>
@@ -4435,13 +4425,13 @@
     <row r="35" spans="1:37" x14ac:dyDescent="0.45">
       <c r="A35" s="4"/>
       <c r="B35" s="4" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="D35" s="4" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="E35" s="4">
         <v>1</v>
@@ -4450,7 +4440,7 @@
         <v>1</v>
       </c>
       <c r="G35" s="4" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="H35" s="4">
         <v>4</v>
@@ -4518,13 +4508,13 @@
     <row r="36" spans="1:37" x14ac:dyDescent="0.45">
       <c r="A36" s="4"/>
       <c r="B36" s="4" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="D36" s="4" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="E36" s="4">
         <v>1</v>
@@ -4533,7 +4523,7 @@
         <v>1</v>
       </c>
       <c r="G36" s="4" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="H36" s="4">
         <v>4</v>
@@ -4601,13 +4591,13 @@
     <row r="37" spans="1:37" x14ac:dyDescent="0.45">
       <c r="A37" s="4"/>
       <c r="B37" s="4" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="D37" s="4" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="E37" s="4">
         <v>1</v>
@@ -4616,7 +4606,7 @@
         <v>1</v>
       </c>
       <c r="G37" s="4" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="H37" s="4">
         <v>4</v>
@@ -4684,13 +4674,13 @@
     <row r="38" spans="1:37" x14ac:dyDescent="0.45">
       <c r="A38" s="4"/>
       <c r="B38" s="4" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="D38" s="4" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="E38" s="4">
         <v>1</v>
@@ -4699,7 +4689,7 @@
         <v>1</v>
       </c>
       <c r="G38" s="4" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="H38" s="4">
         <v>4</v>
@@ -4767,13 +4757,13 @@
     <row r="39" spans="1:37" x14ac:dyDescent="0.45">
       <c r="A39" s="4"/>
       <c r="B39" s="4" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="D39" s="4" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="E39" s="4">
         <v>1</v>
@@ -4782,7 +4772,7 @@
         <v>1</v>
       </c>
       <c r="G39" s="4" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="H39" s="4">
         <v>4</v>
@@ -4850,13 +4840,13 @@
     <row r="40" spans="1:37" x14ac:dyDescent="0.45">
       <c r="A40" s="4"/>
       <c r="B40" s="4" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="D40" s="4" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="E40" s="4">
         <v>1</v>
@@ -4865,7 +4855,7 @@
         <v>1</v>
       </c>
       <c r="G40" s="4" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="H40" s="4">
         <v>4</v>
@@ -4933,13 +4923,13 @@
     <row r="41" spans="1:37" x14ac:dyDescent="0.45">
       <c r="A41" s="4"/>
       <c r="B41" s="4" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="D41" s="4" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="E41" s="4">
         <v>1</v>
@@ -4948,7 +4938,7 @@
         <v>1</v>
       </c>
       <c r="G41" s="4" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="H41" s="4">
         <v>4</v>
@@ -5016,13 +5006,13 @@
     <row r="42" spans="1:37" x14ac:dyDescent="0.45">
       <c r="A42" s="4"/>
       <c r="B42" s="4" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="D42" s="4" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="E42" s="4">
         <v>1</v>
@@ -5031,7 +5021,7 @@
         <v>1</v>
       </c>
       <c r="G42" s="4" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="H42" s="4">
         <v>4</v>
@@ -5099,13 +5089,13 @@
     <row r="43" spans="1:37" x14ac:dyDescent="0.45">
       <c r="A43" s="4"/>
       <c r="B43" s="4" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="D43" s="4" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="E43" s="4">
         <v>1</v>
@@ -5114,7 +5104,7 @@
         <v>1</v>
       </c>
       <c r="G43" s="4" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="H43" s="4">
         <v>4</v>
@@ -5182,13 +5172,13 @@
     <row r="44" spans="1:37" x14ac:dyDescent="0.45">
       <c r="A44" s="4"/>
       <c r="B44" s="4" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="D44" s="4" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="E44" s="4">
         <v>1</v>
@@ -5197,7 +5187,7 @@
         <v>1</v>
       </c>
       <c r="G44" s="4" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="H44" s="4">
         <v>4</v>
@@ -5265,13 +5255,13 @@
     <row r="45" spans="1:37" x14ac:dyDescent="0.45">
       <c r="A45" s="4"/>
       <c r="B45" s="4" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="D45" s="4" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="E45" s="4">
         <v>1</v>
@@ -5280,7 +5270,7 @@
         <v>1</v>
       </c>
       <c r="G45" s="4" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="H45" s="4">
         <v>4</v>
@@ -5348,13 +5338,13 @@
     <row r="46" spans="1:37" x14ac:dyDescent="0.45">
       <c r="A46" s="4"/>
       <c r="B46" s="4" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="D46" s="4" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="E46" s="4">
         <v>1</v>
@@ -5363,7 +5353,7 @@
         <v>1</v>
       </c>
       <c r="G46" s="4" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="H46" s="4">
         <v>4</v>
@@ -5433,13 +5423,13 @@
     <row r="47" spans="1:37" x14ac:dyDescent="0.45">
       <c r="A47" s="4"/>
       <c r="B47" s="4" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="D47" s="4" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="E47" s="4">
         <v>1</v>
@@ -5448,7 +5438,7 @@
         <v>1</v>
       </c>
       <c r="G47" s="4" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="H47" s="4">
         <v>4</v>
@@ -5516,13 +5506,13 @@
     <row r="48" spans="1:37" x14ac:dyDescent="0.45">
       <c r="A48" s="4"/>
       <c r="B48" s="4" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
       <c r="C48" s="4" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="D48" s="4" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="E48" s="4">
         <v>1</v>
@@ -5531,7 +5521,7 @@
         <v>1</v>
       </c>
       <c r="G48" s="4" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="H48" s="4">
         <v>4</v>
@@ -5599,13 +5589,13 @@
     <row r="49" spans="1:37" x14ac:dyDescent="0.45">
       <c r="A49" s="4"/>
       <c r="B49" s="4" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
       <c r="C49" s="4" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="D49" s="4" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="E49" s="4">
         <v>1</v>
@@ -5614,7 +5604,7 @@
         <v>1</v>
       </c>
       <c r="G49" s="4" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="H49" s="4">
         <v>4</v>
@@ -5682,13 +5672,13 @@
     <row r="50" spans="1:37" x14ac:dyDescent="0.45">
       <c r="A50" s="4"/>
       <c r="B50" s="4" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
       <c r="C50" s="4" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="D50" s="4" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="E50" s="4">
         <v>1</v>
@@ -5697,7 +5687,7 @@
         <v>1</v>
       </c>
       <c r="G50" s="4" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="H50" s="4">
         <v>4</v>
@@ -5765,13 +5755,13 @@
     <row r="51" spans="1:37" x14ac:dyDescent="0.45">
       <c r="A51" s="4"/>
       <c r="B51" s="4" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
       <c r="C51" s="4" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="D51" s="4" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="E51" s="4">
         <v>1</v>
@@ -5780,7 +5770,7 @@
         <v>1</v>
       </c>
       <c r="G51" s="4" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="H51" s="4">
         <v>4</v>
@@ -5848,13 +5838,13 @@
     <row r="52" spans="1:37" x14ac:dyDescent="0.45">
       <c r="A52" s="4"/>
       <c r="B52" s="4" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
       <c r="C52" s="4" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="D52" s="4" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="E52" s="4">
         <v>1</v>
@@ -5863,7 +5853,7 @@
         <v>1</v>
       </c>
       <c r="G52" s="4" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="H52" s="4">
         <v>4</v>
@@ -5931,13 +5921,13 @@
     <row r="53" spans="1:37" x14ac:dyDescent="0.45">
       <c r="A53" s="4"/>
       <c r="B53" s="4" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
       <c r="C53" s="4" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="D53" s="4" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="E53" s="4">
         <v>1</v>
@@ -5946,7 +5936,7 @@
         <v>1</v>
       </c>
       <c r="G53" s="4" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="H53" s="4">
         <v>4</v>
@@ -6014,13 +6004,13 @@
     <row r="54" spans="1:37" x14ac:dyDescent="0.45">
       <c r="A54" s="4"/>
       <c r="B54" s="4" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
       <c r="C54" s="4" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="D54" s="4" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="E54" s="4">
         <v>1</v>
@@ -6029,7 +6019,7 @@
         <v>1</v>
       </c>
       <c r="G54" s="4" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="H54" s="4">
         <v>4</v>
@@ -6099,13 +6089,13 @@
     <row r="55" spans="1:37" x14ac:dyDescent="0.45">
       <c r="A55" s="4"/>
       <c r="B55" s="4" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
       <c r="C55" s="4" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="D55" s="4" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="E55" s="4">
         <v>1</v>
@@ -6114,7 +6104,7 @@
         <v>1</v>
       </c>
       <c r="G55" s="4" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="H55" s="4">
         <v>4</v>
@@ -6184,13 +6174,13 @@
     <row r="56" spans="1:37" x14ac:dyDescent="0.45">
       <c r="A56" s="4"/>
       <c r="B56" s="4" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
       <c r="C56" s="4" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="D56" s="4" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="E56" s="4">
         <v>1</v>
@@ -6199,7 +6189,7 @@
         <v>1</v>
       </c>
       <c r="G56" s="4" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="H56" s="4">
         <v>4</v>
@@ -6267,13 +6257,13 @@
     <row r="57" spans="1:37" x14ac:dyDescent="0.45">
       <c r="A57" s="4"/>
       <c r="B57" s="4" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
       <c r="C57" s="4" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="D57" s="4" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="E57" s="4">
         <v>1</v>
@@ -6282,7 +6272,7 @@
         <v>1</v>
       </c>
       <c r="G57" s="4" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="H57" s="4">
         <v>4</v>
@@ -6350,13 +6340,13 @@
     <row r="58" spans="1:37" x14ac:dyDescent="0.45">
       <c r="A58" s="4"/>
       <c r="B58" s="4" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
       <c r="C58" s="4" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="D58" s="4" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="E58" s="4">
         <v>1</v>
@@ -6365,7 +6355,7 @@
         <v>1</v>
       </c>
       <c r="G58" s="4" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="H58" s="4">
         <v>4</v>
@@ -6433,13 +6423,13 @@
     <row r="59" spans="1:37" x14ac:dyDescent="0.45">
       <c r="A59" s="4"/>
       <c r="B59" s="4" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
       <c r="C59" s="4" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="D59" s="4" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="E59" s="4">
         <v>1</v>
@@ -6448,7 +6438,7 @@
         <v>1</v>
       </c>
       <c r="G59" s="4" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="H59" s="4">
         <v>4</v>
@@ -6516,13 +6506,13 @@
     <row r="60" spans="1:37" x14ac:dyDescent="0.45">
       <c r="A60" s="4"/>
       <c r="B60" s="4" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
       <c r="C60" s="4" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="D60" s="4" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="E60" s="4">
         <v>1</v>
@@ -6531,7 +6521,7 @@
         <v>1</v>
       </c>
       <c r="G60" s="4" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="H60" s="4">
         <v>4</v>
@@ -6599,13 +6589,13 @@
     <row r="61" spans="1:37" x14ac:dyDescent="0.45">
       <c r="A61" s="4"/>
       <c r="B61" s="4" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
       <c r="C61" s="4" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="D61" s="4" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="E61" s="4">
         <v>1</v>
@@ -6614,7 +6604,7 @@
         <v>1</v>
       </c>
       <c r="G61" s="4" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="H61" s="4">
         <v>4</v>
@@ -6684,13 +6674,13 @@
     <row r="62" spans="1:37" x14ac:dyDescent="0.45">
       <c r="A62" s="4"/>
       <c r="B62" s="4" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
       <c r="C62" s="4" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="D62" s="4" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="E62" s="4">
         <v>1</v>
@@ -6699,7 +6689,7 @@
         <v>1</v>
       </c>
       <c r="G62" s="4" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="H62" s="4">
         <v>4</v>
@@ -6763,12 +6753,9 @@
       <c r="AK62" s="4"/>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="AF4" r:id="rId1" display="../../../../../../../:i:/g/personal/fernando_brefere_com_br/EckQHxh9ywZLs543cFd570cBTVoQq-9gsOR3Cltq1fa46A?e=V7BxnI" xr:uid="{6578994B-5733-4280-906F-F7ED81A75E47}"/>
-  </hyperlinks>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Atualização de dados e imagens
</commit_message>
<xml_diff>
--- a/data/Base de levantamento Sphenophorus.xlsx
+++ b/data/Base de levantamento Sphenophorus.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://breferecombr-my.sharepoint.com/personal/fernando_brefere_com_br/Documents/01_P.A.R.A/01.Projetos/projeto_sphenophorus/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="75" documentId="8_{D20646F8-C54A-4EE1-997D-BABB7AF84F48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E0A52029-53EA-4176-B6C1-1C6D6EC7169D}"/>
+  <xr:revisionPtr revIDLastSave="114" documentId="8_{D20646F8-C54A-4EE1-997D-BABB7AF84F48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FED1C647-36C3-4B2E-B701-1B96B9D21E52}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="11475" xr2:uid="{D8EDB14A-D587-475B-A286-93234BB649C9}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="530" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="570" uniqueCount="76">
   <si>
     <t>Indice de aplicação:</t>
   </si>
@@ -237,6 +237,33 @@
   </si>
   <si>
     <t>Foto 6</t>
+  </si>
+  <si>
+    <t>Fernando Brefere</t>
+  </si>
+  <si>
+    <t>Fazenda Brefere</t>
+  </si>
+  <si>
+    <t>Penapolis</t>
+  </si>
+  <si>
+    <t>CTC4</t>
+  </si>
+  <si>
+    <t>Plantio</t>
+  </si>
+  <si>
+    <t>Curbix 6,0</t>
+  </si>
+  <si>
+    <t>Curbix7,0</t>
+  </si>
+  <si>
+    <t>Curbix8,0</t>
+  </si>
+  <si>
+    <t>Curbix9,0</t>
   </si>
 </sst>
 </file>
@@ -313,7 +340,7 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -326,6 +353,9 @@
     <xf numFmtId="10" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2"/>
     <xf numFmtId="10" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hiperlink" xfId="2" builtinId="8"/>
@@ -1150,8 +1180,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{33C4D4BE-CDE2-43A0-BDF8-CBEB65C4D1E0}" name="fFichaSphenophorus" displayName="fFichaSphenophorus" ref="A2:AK62" totalsRowShown="0" dataDxfId="37">
-  <autoFilter ref="A2:AK62" xr:uid="{F72C1B53-5DC3-4CC8-BF06-EDFFB5A060DD}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{33C4D4BE-CDE2-43A0-BDF8-CBEB65C4D1E0}" name="fFichaSphenophorus" displayName="fFichaSphenophorus" ref="A2:AK67" totalsRowShown="0" dataDxfId="37">
+  <autoFilter ref="A2:AK67" xr:uid="{F72C1B53-5DC3-4CC8-BF06-EDFFB5A060DD}"/>
   <tableColumns count="37">
     <tableColumn id="28" xr3:uid="{E06CCBC7-1FC5-40F5-9A03-0510EA2F36B5}" name="Cod_Cliente" dataDxfId="36"/>
     <tableColumn id="1" xr3:uid="{1A6942EC-A856-45EB-B1CD-A7D98DE0FC50}" name="Nome_Cliente" dataDxfId="35"/>
@@ -1514,10 +1544,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7FB08C5-DA3B-4BF7-B0CE-50F695BC8261}">
-  <dimension ref="A1:AK62"/>
+  <dimension ref="A1:AK67"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="AF1" workbookViewId="0">
-      <selection activeCell="AF9" sqref="AF9"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A47" workbookViewId="0">
+      <selection activeCell="G60" sqref="G60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -6752,6 +6782,436 @@
       <c r="AJ62" s="4"/>
       <c r="AK62" s="4"/>
     </row>
+    <row r="63" spans="1:37" x14ac:dyDescent="0.45">
+      <c r="A63" s="10">
+        <v>304050</v>
+      </c>
+      <c r="B63" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="C63" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="D63" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="E63" s="10">
+        <v>1</v>
+      </c>
+      <c r="F63" s="10">
+        <v>2</v>
+      </c>
+      <c r="G63" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="H63" s="10">
+        <v>2</v>
+      </c>
+      <c r="I63" s="10"/>
+      <c r="J63" s="10"/>
+      <c r="K63" s="5">
+        <v>45199</v>
+      </c>
+      <c r="L63" s="11">
+        <v>200</v>
+      </c>
+      <c r="M63" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="N63" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="O63" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="P63" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="Q63" s="11">
+        <v>1</v>
+      </c>
+      <c r="R63" s="10"/>
+      <c r="S63" s="10">
+        <v>1</v>
+      </c>
+      <c r="T63" s="10">
+        <v>1</v>
+      </c>
+      <c r="U63" s="12">
+        <v>45658</v>
+      </c>
+      <c r="V63" s="4">
+        <v>86</v>
+      </c>
+      <c r="W63" s="4">
+        <v>12</v>
+      </c>
+      <c r="X63" s="9">
+        <f>(W63/V63)</f>
+        <v>0.13953488372093023</v>
+      </c>
+      <c r="Y63" s="4">
+        <v>0</v>
+      </c>
+      <c r="Z63" s="4"/>
+      <c r="AA63" s="4"/>
+      <c r="AB63" s="4"/>
+      <c r="AC63" s="4"/>
+      <c r="AD63" s="4"/>
+      <c r="AE63" s="4">
+        <v>0</v>
+      </c>
+      <c r="AF63" s="4"/>
+      <c r="AG63" s="4"/>
+      <c r="AH63" s="4"/>
+      <c r="AI63" s="4"/>
+      <c r="AJ63" s="4"/>
+      <c r="AK63" s="4"/>
+    </row>
+    <row r="64" spans="1:37" x14ac:dyDescent="0.45">
+      <c r="A64" s="10">
+        <v>304050</v>
+      </c>
+      <c r="B64" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="C64" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="D64" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="E64" s="10">
+        <v>1</v>
+      </c>
+      <c r="F64" s="10">
+        <v>2</v>
+      </c>
+      <c r="G64" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="H64" s="10">
+        <v>2</v>
+      </c>
+      <c r="I64" s="10"/>
+      <c r="J64" s="10"/>
+      <c r="K64" s="5">
+        <v>45199</v>
+      </c>
+      <c r="L64" s="11">
+        <v>200</v>
+      </c>
+      <c r="M64" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="N64" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="O64" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="P64" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="Q64" s="11">
+        <v>2</v>
+      </c>
+      <c r="R64" s="10"/>
+      <c r="S64" s="10">
+        <v>2</v>
+      </c>
+      <c r="T64" s="10">
+        <v>2</v>
+      </c>
+      <c r="U64" s="12">
+        <v>45659</v>
+      </c>
+      <c r="V64" s="4">
+        <v>86</v>
+      </c>
+      <c r="W64" s="4">
+        <v>12</v>
+      </c>
+      <c r="X64" s="9">
+        <f>(W64/V64)</f>
+        <v>0.13953488372093023</v>
+      </c>
+      <c r="Y64" s="4">
+        <v>0</v>
+      </c>
+      <c r="Z64" s="4"/>
+      <c r="AA64" s="4"/>
+      <c r="AB64" s="4"/>
+      <c r="AC64" s="4"/>
+      <c r="AD64" s="4"/>
+      <c r="AE64" s="4">
+        <v>0</v>
+      </c>
+      <c r="AF64" s="4"/>
+      <c r="AG64" s="4"/>
+      <c r="AH64" s="4"/>
+      <c r="AI64" s="4"/>
+      <c r="AJ64" s="4"/>
+      <c r="AK64" s="4"/>
+    </row>
+    <row r="65" spans="1:37" x14ac:dyDescent="0.45">
+      <c r="A65" s="10">
+        <v>304050</v>
+      </c>
+      <c r="B65" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="C65" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="D65" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="E65" s="10">
+        <v>1</v>
+      </c>
+      <c r="F65" s="10">
+        <v>2</v>
+      </c>
+      <c r="G65" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="H65" s="10">
+        <v>2</v>
+      </c>
+      <c r="I65" s="10"/>
+      <c r="J65" s="10"/>
+      <c r="K65" s="5">
+        <v>45199</v>
+      </c>
+      <c r="L65" s="11">
+        <v>200</v>
+      </c>
+      <c r="M65" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="N65" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="O65" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="P65" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="Q65" s="11">
+        <v>3</v>
+      </c>
+      <c r="R65" s="10"/>
+      <c r="S65" s="10">
+        <v>3</v>
+      </c>
+      <c r="T65" s="10">
+        <v>3</v>
+      </c>
+      <c r="U65" s="12">
+        <v>45660</v>
+      </c>
+      <c r="V65" s="4">
+        <v>77</v>
+      </c>
+      <c r="W65" s="4">
+        <v>10</v>
+      </c>
+      <c r="X65" s="9">
+        <f>(W65/V65)</f>
+        <v>0.12987012987012986</v>
+      </c>
+      <c r="Y65" s="4">
+        <v>0</v>
+      </c>
+      <c r="Z65" s="4"/>
+      <c r="AA65" s="4"/>
+      <c r="AB65" s="4"/>
+      <c r="AC65" s="4"/>
+      <c r="AD65" s="4"/>
+      <c r="AE65" s="4">
+        <v>0</v>
+      </c>
+      <c r="AF65" s="4"/>
+      <c r="AG65" s="4"/>
+      <c r="AH65" s="4"/>
+      <c r="AI65" s="4"/>
+      <c r="AJ65" s="4"/>
+      <c r="AK65" s="4"/>
+    </row>
+    <row r="66" spans="1:37" x14ac:dyDescent="0.45">
+      <c r="A66" s="10">
+        <v>304050</v>
+      </c>
+      <c r="B66" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="C66" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="D66" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="E66" s="10">
+        <v>1</v>
+      </c>
+      <c r="F66" s="10">
+        <v>2</v>
+      </c>
+      <c r="G66" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="H66" s="10">
+        <v>2</v>
+      </c>
+      <c r="I66" s="10"/>
+      <c r="J66" s="10"/>
+      <c r="K66" s="5">
+        <v>45199</v>
+      </c>
+      <c r="L66" s="11">
+        <v>200</v>
+      </c>
+      <c r="M66" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="N66" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="O66" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="P66" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="Q66" s="11">
+        <v>4</v>
+      </c>
+      <c r="R66" s="10"/>
+      <c r="S66" s="10">
+        <v>4</v>
+      </c>
+      <c r="T66" s="10">
+        <v>4</v>
+      </c>
+      <c r="U66" s="12">
+        <v>45661</v>
+      </c>
+      <c r="V66" s="4">
+        <v>96</v>
+      </c>
+      <c r="W66" s="4">
+        <v>22</v>
+      </c>
+      <c r="X66" s="9">
+        <f>(W66/V66)</f>
+        <v>0.22916666666666666</v>
+      </c>
+      <c r="Y66" s="4">
+        <v>2</v>
+      </c>
+      <c r="Z66" s="4"/>
+      <c r="AA66" s="4"/>
+      <c r="AB66" s="4"/>
+      <c r="AC66" s="4">
+        <v>2</v>
+      </c>
+      <c r="AD66" s="4"/>
+      <c r="AE66" s="4">
+        <v>4</v>
+      </c>
+      <c r="AF66" s="4"/>
+      <c r="AG66" s="4"/>
+      <c r="AH66" s="4"/>
+      <c r="AI66" s="4"/>
+      <c r="AJ66" s="4"/>
+      <c r="AK66" s="4"/>
+    </row>
+    <row r="67" spans="1:37" x14ac:dyDescent="0.45">
+      <c r="A67" s="10">
+        <v>304050</v>
+      </c>
+      <c r="B67" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="C67" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="D67" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="E67" s="10">
+        <v>1</v>
+      </c>
+      <c r="F67" s="10">
+        <v>2</v>
+      </c>
+      <c r="G67" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="H67" s="10">
+        <v>2</v>
+      </c>
+      <c r="I67" s="10"/>
+      <c r="J67" s="10"/>
+      <c r="K67" s="5">
+        <v>45199</v>
+      </c>
+      <c r="L67" s="11">
+        <v>200</v>
+      </c>
+      <c r="M67" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="N67" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="O67" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="P67" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q67" s="11">
+        <v>5</v>
+      </c>
+      <c r="R67" s="10"/>
+      <c r="S67" s="10">
+        <v>5</v>
+      </c>
+      <c r="T67" s="10">
+        <v>5</v>
+      </c>
+      <c r="U67" s="12">
+        <v>45662</v>
+      </c>
+      <c r="V67" s="4">
+        <v>100</v>
+      </c>
+      <c r="W67" s="4">
+        <v>24</v>
+      </c>
+      <c r="X67" s="9">
+        <f>(W67/V67)</f>
+        <v>0.24</v>
+      </c>
+      <c r="Y67" s="4">
+        <v>0</v>
+      </c>
+      <c r="Z67" s="4"/>
+      <c r="AA67" s="4"/>
+      <c r="AB67" s="4"/>
+      <c r="AC67" s="4"/>
+      <c r="AD67" s="4"/>
+      <c r="AE67" s="4"/>
+      <c r="AF67" s="4"/>
+      <c r="AG67" s="4"/>
+      <c r="AH67" s="4"/>
+      <c r="AI67" s="4"/>
+      <c r="AJ67" s="4"/>
+      <c r="AK67" s="4"/>
+    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <tableParts count="1">

</xml_diff>

<commit_message>
Corrige caminho da planilha para funcionar no Streamlit Cloud
</commit_message>
<xml_diff>
--- a/data/Base de levantamento Sphenophorus.xlsx
+++ b/data/Base de levantamento Sphenophorus.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://breferecombr-my.sharepoint.com/personal/fernando_brefere_com_br/Documents/01_P.A.R.A/01.Projetos/projeto_sphenophorus/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="114" documentId="8_{D20646F8-C54A-4EE1-997D-BABB7AF84F48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FED1C647-36C3-4B2E-B701-1B96B9D21E52}"/>
+  <xr:revisionPtr revIDLastSave="140" documentId="8_{D20646F8-C54A-4EE1-997D-BABB7AF84F48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{295D5190-9774-4355-A337-4878EC06836C}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="11475" xr2:uid="{D8EDB14A-D587-475B-A286-93234BB649C9}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="570" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="580" uniqueCount="83">
   <si>
     <t>Indice de aplicação:</t>
   </si>
@@ -264,6 +264,27 @@
   </si>
   <si>
     <t>Curbix9,0</t>
+  </si>
+  <si>
+    <t>Cliente Simulado</t>
+  </si>
+  <si>
+    <t>Fazenda Teste</t>
+  </si>
+  <si>
+    <t>Tratamento XYZ</t>
+  </si>
+  <si>
+    <t>C:\Users\fatbr\OneDrive\Documents\GitHub\projeto_sphenophorus\fotos_sphenophorus\Teste1.png</t>
+  </si>
+  <si>
+    <t>C:\Users\fatbr\OneDrive\Documents\GitHub\projeto_sphenophorus\fotos_sphenophorus\Teste2.png</t>
+  </si>
+  <si>
+    <t>Teste1</t>
+  </si>
+  <si>
+    <t>Teste 2</t>
   </si>
 </sst>
 </file>
@@ -354,8 +375,8 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2"/>
     <xf numFmtId="10" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hiperlink" xfId="2" builtinId="8"/>
@@ -1180,8 +1201,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{33C4D4BE-CDE2-43A0-BDF8-CBEB65C4D1E0}" name="fFichaSphenophorus" displayName="fFichaSphenophorus" ref="A2:AK67" totalsRowShown="0" dataDxfId="37">
-  <autoFilter ref="A2:AK67" xr:uid="{F72C1B53-5DC3-4CC8-BF06-EDFFB5A060DD}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{33C4D4BE-CDE2-43A0-BDF8-CBEB65C4D1E0}" name="fFichaSphenophorus" displayName="fFichaSphenophorus" ref="A2:AK68" totalsRowShown="0" dataDxfId="37">
+  <autoFilter ref="A2:AK68" xr:uid="{F72C1B53-5DC3-4CC8-BF06-EDFFB5A060DD}"/>
   <tableColumns count="37">
     <tableColumn id="28" xr3:uid="{E06CCBC7-1FC5-40F5-9A03-0510EA2F36B5}" name="Cod_Cliente" dataDxfId="36"/>
     <tableColumn id="1" xr3:uid="{1A6942EC-A856-45EB-B1CD-A7D98DE0FC50}" name="Nome_Cliente" dataDxfId="35"/>
@@ -1544,18 +1565,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7FB08C5-DA3B-4BF7-B0CE-50F695BC8261}">
-  <dimension ref="A1:AK67"/>
+  <dimension ref="A1:AK68"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A47" workbookViewId="0">
-      <selection activeCell="G60" sqref="G60"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="AE53" workbookViewId="0">
+      <selection activeCell="AF58" sqref="AF58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="2" width="17.46484375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.46484375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.19921875" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.1328125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="15.86328125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="13.46484375" bestFit="1" customWidth="1"/>
@@ -1578,7 +1598,7 @@
     <col min="28" max="28" width="13.19921875" bestFit="1" customWidth="1"/>
     <col min="29" max="29" width="19.53125" bestFit="1" customWidth="1"/>
     <col min="30" max="31" width="22.19921875" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="96.46484375" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="80.73046875" bestFit="1" customWidth="1"/>
     <col min="33" max="33" width="12.19921875" bestFit="1" customWidth="1"/>
     <col min="34" max="34" width="22.06640625" bestFit="1" customWidth="1"/>
     <col min="35" max="35" width="12.19921875" bestFit="1" customWidth="1"/>
@@ -6783,61 +6803,61 @@
       <c r="AK62" s="4"/>
     </row>
     <row r="63" spans="1:37" x14ac:dyDescent="0.45">
-      <c r="A63" s="10">
+      <c r="A63" s="4">
         <v>304050</v>
       </c>
-      <c r="B63" s="10" t="s">
+      <c r="B63" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="C63" s="10" t="s">
+      <c r="C63" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="D63" s="10" t="s">
+      <c r="D63" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="E63" s="10">
-        <v>1</v>
-      </c>
-      <c r="F63" s="10">
-        <v>2</v>
-      </c>
-      <c r="G63" s="10" t="s">
+      <c r="E63" s="4">
+        <v>1</v>
+      </c>
+      <c r="F63" s="4">
+        <v>2</v>
+      </c>
+      <c r="G63" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="H63" s="10">
-        <v>2</v>
-      </c>
-      <c r="I63" s="10"/>
-      <c r="J63" s="10"/>
+      <c r="H63" s="4">
+        <v>2</v>
+      </c>
+      <c r="I63" s="4"/>
+      <c r="J63" s="4"/>
       <c r="K63" s="5">
         <v>45199</v>
       </c>
-      <c r="L63" s="11">
+      <c r="L63" s="6">
         <v>200</v>
       </c>
-      <c r="M63" s="11" t="s">
+      <c r="M63" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="N63" s="11" t="s">
+      <c r="N63" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="O63" s="11" t="s">
+      <c r="O63" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="P63" s="10" t="s">
+      <c r="P63" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="Q63" s="11">
-        <v>1</v>
-      </c>
-      <c r="R63" s="10"/>
-      <c r="S63" s="10">
-        <v>1</v>
-      </c>
-      <c r="T63" s="10">
-        <v>1</v>
-      </c>
-      <c r="U63" s="12">
+      <c r="Q63" s="6">
+        <v>1</v>
+      </c>
+      <c r="R63" s="4"/>
+      <c r="S63" s="4">
+        <v>1</v>
+      </c>
+      <c r="T63" s="4">
+        <v>1</v>
+      </c>
+      <c r="U63" s="5">
         <v>45658</v>
       </c>
       <c r="V63" s="4">
@@ -6869,61 +6889,61 @@
       <c r="AK63" s="4"/>
     </row>
     <row r="64" spans="1:37" x14ac:dyDescent="0.45">
-      <c r="A64" s="10">
+      <c r="A64" s="4">
         <v>304050</v>
       </c>
-      <c r="B64" s="10" t="s">
+      <c r="B64" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="C64" s="10" t="s">
+      <c r="C64" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="D64" s="10" t="s">
+      <c r="D64" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="E64" s="10">
-        <v>1</v>
-      </c>
-      <c r="F64" s="10">
-        <v>2</v>
-      </c>
-      <c r="G64" s="10" t="s">
+      <c r="E64" s="4">
+        <v>1</v>
+      </c>
+      <c r="F64" s="4">
+        <v>2</v>
+      </c>
+      <c r="G64" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="H64" s="10">
-        <v>2</v>
-      </c>
-      <c r="I64" s="10"/>
-      <c r="J64" s="10"/>
+      <c r="H64" s="4">
+        <v>2</v>
+      </c>
+      <c r="I64" s="4"/>
+      <c r="J64" s="4"/>
       <c r="K64" s="5">
         <v>45199</v>
       </c>
-      <c r="L64" s="11">
+      <c r="L64" s="6">
         <v>200</v>
       </c>
-      <c r="M64" s="11" t="s">
+      <c r="M64" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="N64" s="11" t="s">
+      <c r="N64" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="O64" s="11" t="s">
+      <c r="O64" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="P64" s="10" t="s">
+      <c r="P64" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="Q64" s="11">
-        <v>2</v>
-      </c>
-      <c r="R64" s="10"/>
-      <c r="S64" s="10">
-        <v>2</v>
-      </c>
-      <c r="T64" s="10">
-        <v>2</v>
-      </c>
-      <c r="U64" s="12">
+      <c r="Q64" s="6">
+        <v>2</v>
+      </c>
+      <c r="R64" s="4"/>
+      <c r="S64" s="4">
+        <v>2</v>
+      </c>
+      <c r="T64" s="4">
+        <v>2</v>
+      </c>
+      <c r="U64" s="5">
         <v>45659</v>
       </c>
       <c r="V64" s="4">
@@ -6955,61 +6975,61 @@
       <c r="AK64" s="4"/>
     </row>
     <row r="65" spans="1:37" x14ac:dyDescent="0.45">
-      <c r="A65" s="10">
+      <c r="A65" s="4">
         <v>304050</v>
       </c>
-      <c r="B65" s="10" t="s">
+      <c r="B65" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="C65" s="10" t="s">
+      <c r="C65" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="D65" s="10" t="s">
+      <c r="D65" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="E65" s="10">
-        <v>1</v>
-      </c>
-      <c r="F65" s="10">
-        <v>2</v>
-      </c>
-      <c r="G65" s="10" t="s">
+      <c r="E65" s="4">
+        <v>1</v>
+      </c>
+      <c r="F65" s="4">
+        <v>2</v>
+      </c>
+      <c r="G65" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="H65" s="10">
-        <v>2</v>
-      </c>
-      <c r="I65" s="10"/>
-      <c r="J65" s="10"/>
+      <c r="H65" s="4">
+        <v>2</v>
+      </c>
+      <c r="I65" s="4"/>
+      <c r="J65" s="4"/>
       <c r="K65" s="5">
         <v>45199</v>
       </c>
-      <c r="L65" s="11">
+      <c r="L65" s="6">
         <v>200</v>
       </c>
-      <c r="M65" s="11" t="s">
+      <c r="M65" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="N65" s="11" t="s">
+      <c r="N65" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="O65" s="11" t="s">
+      <c r="O65" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="P65" s="10" t="s">
+      <c r="P65" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="Q65" s="11">
-        <v>3</v>
-      </c>
-      <c r="R65" s="10"/>
-      <c r="S65" s="10">
-        <v>3</v>
-      </c>
-      <c r="T65" s="10">
-        <v>3</v>
-      </c>
-      <c r="U65" s="12">
+      <c r="Q65" s="6">
+        <v>3</v>
+      </c>
+      <c r="R65" s="4"/>
+      <c r="S65" s="4">
+        <v>3</v>
+      </c>
+      <c r="T65" s="4">
+        <v>3</v>
+      </c>
+      <c r="U65" s="5">
         <v>45660</v>
       </c>
       <c r="V65" s="4">
@@ -7041,61 +7061,61 @@
       <c r="AK65" s="4"/>
     </row>
     <row r="66" spans="1:37" x14ac:dyDescent="0.45">
-      <c r="A66" s="10">
+      <c r="A66" s="4">
         <v>304050</v>
       </c>
-      <c r="B66" s="10" t="s">
+      <c r="B66" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="C66" s="10" t="s">
+      <c r="C66" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="D66" s="10" t="s">
+      <c r="D66" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="E66" s="10">
-        <v>1</v>
-      </c>
-      <c r="F66" s="10">
-        <v>2</v>
-      </c>
-      <c r="G66" s="10" t="s">
+      <c r="E66" s="4">
+        <v>1</v>
+      </c>
+      <c r="F66" s="4">
+        <v>2</v>
+      </c>
+      <c r="G66" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="H66" s="10">
-        <v>2</v>
-      </c>
-      <c r="I66" s="10"/>
-      <c r="J66" s="10"/>
+      <c r="H66" s="4">
+        <v>2</v>
+      </c>
+      <c r="I66" s="4"/>
+      <c r="J66" s="4"/>
       <c r="K66" s="5">
         <v>45199</v>
       </c>
-      <c r="L66" s="11">
+      <c r="L66" s="6">
         <v>200</v>
       </c>
-      <c r="M66" s="11" t="s">
+      <c r="M66" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="N66" s="11" t="s">
+      <c r="N66" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="O66" s="11" t="s">
+      <c r="O66" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="P66" s="10" t="s">
+      <c r="P66" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="Q66" s="11">
+      <c r="Q66" s="6">
         <v>4</v>
       </c>
-      <c r="R66" s="10"/>
-      <c r="S66" s="10">
+      <c r="R66" s="4"/>
+      <c r="S66" s="4">
         <v>4</v>
       </c>
-      <c r="T66" s="10">
+      <c r="T66" s="4">
         <v>4</v>
       </c>
-      <c r="U66" s="12">
+      <c r="U66" s="5">
         <v>45661</v>
       </c>
       <c r="V66" s="4">
@@ -7129,61 +7149,61 @@
       <c r="AK66" s="4"/>
     </row>
     <row r="67" spans="1:37" x14ac:dyDescent="0.45">
-      <c r="A67" s="10">
+      <c r="A67" s="4">
         <v>304050</v>
       </c>
-      <c r="B67" s="10" t="s">
+      <c r="B67" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="C67" s="10" t="s">
+      <c r="C67" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="D67" s="10" t="s">
+      <c r="D67" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="E67" s="10">
-        <v>1</v>
-      </c>
-      <c r="F67" s="10">
-        <v>2</v>
-      </c>
-      <c r="G67" s="10" t="s">
+      <c r="E67" s="4">
+        <v>1</v>
+      </c>
+      <c r="F67" s="4">
+        <v>2</v>
+      </c>
+      <c r="G67" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="H67" s="10">
-        <v>2</v>
-      </c>
-      <c r="I67" s="10"/>
-      <c r="J67" s="10"/>
+      <c r="H67" s="4">
+        <v>2</v>
+      </c>
+      <c r="I67" s="4"/>
+      <c r="J67" s="4"/>
       <c r="K67" s="5">
         <v>45199</v>
       </c>
-      <c r="L67" s="11">
+      <c r="L67" s="6">
         <v>200</v>
       </c>
-      <c r="M67" s="11" t="s">
+      <c r="M67" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="N67" s="11" t="s">
+      <c r="N67" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="O67" s="11" t="s">
+      <c r="O67" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="P67" s="10" t="s">
+      <c r="P67" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="Q67" s="11">
+      <c r="Q67" s="6">
         <v>5</v>
       </c>
-      <c r="R67" s="10"/>
-      <c r="S67" s="10">
+      <c r="R67" s="4"/>
+      <c r="S67" s="4">
         <v>5</v>
       </c>
-      <c r="T67" s="10">
+      <c r="T67" s="4">
         <v>5</v>
       </c>
-      <c r="U67" s="12">
+      <c r="U67" s="5">
         <v>45662</v>
       </c>
       <c r="V67" s="4">
@@ -7212,6 +7232,86 @@
       <c r="AJ67" s="4"/>
       <c r="AK67" s="4"/>
     </row>
+    <row r="68" spans="1:37" x14ac:dyDescent="0.45">
+      <c r="A68" s="10">
+        <v>999</v>
+      </c>
+      <c r="B68" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="C68" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="D68" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="E68" s="4">
+        <v>1</v>
+      </c>
+      <c r="F68" s="4">
+        <v>2</v>
+      </c>
+      <c r="G68" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="H68" s="4">
+        <v>2</v>
+      </c>
+      <c r="I68" s="10"/>
+      <c r="J68" s="10"/>
+      <c r="K68" s="10"/>
+      <c r="L68" s="12"/>
+      <c r="M68" s="12"/>
+      <c r="N68" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="O68" s="12"/>
+      <c r="P68" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="Q68" s="12">
+        <v>4.2</v>
+      </c>
+      <c r="R68" s="10"/>
+      <c r="S68" s="10"/>
+      <c r="T68" s="10"/>
+      <c r="U68" s="11">
+        <v>45627</v>
+      </c>
+      <c r="V68" s="10">
+        <v>50</v>
+      </c>
+      <c r="W68" s="10">
+        <v>10</v>
+      </c>
+      <c r="X68" s="9">
+        <f>(W68/V68)</f>
+        <v>0.2</v>
+      </c>
+      <c r="Y68" s="10">
+        <v>30</v>
+      </c>
+      <c r="Z68" s="10"/>
+      <c r="AA68" s="10"/>
+      <c r="AB68" s="10"/>
+      <c r="AC68" s="10"/>
+      <c r="AD68" s="10"/>
+      <c r="AE68" s="10"/>
+      <c r="AF68" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="AG68" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="AH68" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="AI68" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="AJ68" s="10"/>
+      <c r="AK68" s="10"/>
+    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <tableParts count="1">

</xml_diff>

<commit_message>
atualização de tipo de foto
</commit_message>
<xml_diff>
--- a/data/Base de levantamento Sphenophorus.xlsx
+++ b/data/Base de levantamento Sphenophorus.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fatbr\OneDrive\Documents\GitHub\projeto_sphenophorus\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F385451-066B-4F9A-A299-7AD1E86E2449}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3184E56D-2DBF-4DCE-8F2B-1401E3232C10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="11475" xr2:uid="{D8EDB14A-D587-475B-A286-93234BB649C9}"/>
   </bookViews>
@@ -245,30 +245,6 @@
     <t>Teste 2</t>
   </si>
   <si>
-    <t>Foto1</t>
-  </si>
-  <si>
-    <t>Foto2</t>
-  </si>
-  <si>
-    <t>Foto3</t>
-  </si>
-  <si>
-    <t>Foto4</t>
-  </si>
-  <si>
-    <t>Foto5</t>
-  </si>
-  <si>
-    <t>Foto6</t>
-  </si>
-  <si>
-    <t>Foto7</t>
-  </si>
-  <si>
-    <t>Foto8</t>
-  </si>
-  <si>
     <t>Teste2</t>
   </si>
   <si>
@@ -285,6 +261,30 @@
   </si>
   <si>
     <t>Guilherme Lacava Teste</t>
+  </si>
+  <si>
+    <t>Foto1.jpg</t>
+  </si>
+  <si>
+    <t>Foto2.jpg</t>
+  </si>
+  <si>
+    <t>Foto3.jpg</t>
+  </si>
+  <si>
+    <t>Foto4.jpg</t>
+  </si>
+  <si>
+    <t>Foto5.jpg</t>
+  </si>
+  <si>
+    <t>Foto6.jpg</t>
+  </si>
+  <si>
+    <t>Foto7.jpg</t>
+  </si>
+  <si>
+    <t>Foto8.jpg</t>
   </si>
 </sst>
 </file>
@@ -367,7 +367,7 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -380,7 +380,6 @@
     <xf numFmtId="10" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2"/>
     <xf numFmtId="10" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hiperlink" xfId="2" builtinId="8"/>
@@ -1571,8 +1570,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7FB08C5-DA3B-4BF7-B0CE-50F695BC8261}">
   <dimension ref="A1:AK69"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A50" workbookViewId="0">
-      <selection activeCell="A69" sqref="A69"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="AD61" workbookViewId="0">
+      <selection activeCell="AF72" sqref="AF72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1810,7 +1809,7 @@
         <v>1</v>
       </c>
       <c r="AF3" s="8" t="s">
-        <v>69</v>
+        <v>75</v>
       </c>
       <c r="AG3" s="4" t="s">
         <v>67</v>
@@ -1899,10 +1898,10 @@
         <v>2</v>
       </c>
       <c r="AF4" s="8" t="s">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="AG4" s="4" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="AH4" s="4"/>
       <c r="AI4" s="4"/>
@@ -1988,10 +1987,10 @@
         <v>2</v>
       </c>
       <c r="AF5" s="8" t="s">
-        <v>71</v>
+        <v>77</v>
       </c>
       <c r="AG5" s="4" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="AH5" s="4"/>
       <c r="AI5" s="4"/>
@@ -2077,10 +2076,10 @@
         <v>4</v>
       </c>
       <c r="AF6" s="8" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
       <c r="AG6" s="4" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="AH6" s="4"/>
       <c r="AI6" s="4"/>
@@ -2166,10 +2165,10 @@
         <v>2</v>
       </c>
       <c r="AF7" s="8" t="s">
-        <v>73</v>
+        <v>79</v>
       </c>
       <c r="AG7" s="4" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="AH7" s="8"/>
       <c r="AI7" s="4"/>
@@ -2255,10 +2254,10 @@
         <v>4</v>
       </c>
       <c r="AF8" s="8" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="AG8" s="4" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="AH8" s="4"/>
       <c r="AI8" s="4"/>
@@ -7302,13 +7301,13 @@
       <c r="AD68" s="4"/>
       <c r="AE68" s="4"/>
       <c r="AF68" s="4" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="AG68" s="4" t="s">
         <v>67</v>
       </c>
       <c r="AH68" s="4" t="s">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="AI68" s="4" t="s">
         <v>68</v>
@@ -7317,11 +7316,11 @@
       <c r="AK68" s="4"/>
     </row>
     <row r="69" spans="1:37" x14ac:dyDescent="0.45">
-      <c r="A69" s="10">
+      <c r="A69" s="4">
         <v>9990</v>
       </c>
-      <c r="B69" s="10" t="s">
-        <v>82</v>
+      <c r="B69" s="4" t="s">
+        <v>74</v>
       </c>
       <c r="C69" s="4" t="s">
         <v>65</v>
@@ -7382,13 +7381,13 @@
       <c r="AD69" s="4"/>
       <c r="AE69" s="4"/>
       <c r="AF69" s="4" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="AG69" s="4" t="s">
         <v>67</v>
       </c>
       <c r="AH69" s="4" t="s">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="AI69" s="4" t="s">
         <v>68</v>

</xml_diff>

<commit_message>
atualizar tipo de imagem
</commit_message>
<xml_diff>
--- a/data/Base de levantamento Sphenophorus.xlsx
+++ b/data/Base de levantamento Sphenophorus.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fatbr\OneDrive\Documents\GitHub\projeto_sphenophorus\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{226C0B36-E92B-441E-A83B-374C96B336EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{791FFD84-1BAD-45B7-9362-9A838A621C9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="11475" xr2:uid="{D8EDB14A-D587-475B-A286-93234BB649C9}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="590" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="590" uniqueCount="83">
   <si>
     <t>Indice de aplicação:</t>
   </si>
@@ -263,9 +263,6 @@
     <t>Guilherme Lacava Teste</t>
   </si>
   <si>
-    <t>Foto1.jpg</t>
-  </si>
-  <si>
     <t>Foto2.jpg</t>
   </si>
   <si>
@@ -281,13 +278,13 @@
     <t>Foto6.jpg</t>
   </si>
   <si>
-    <t>Foto7.jpg</t>
-  </si>
-  <si>
-    <t>Foto8.jpg</t>
-  </si>
-  <si>
-    <t>https://github.com/fatbrefere/projeto_sphenophorus/blob/main/fotos_sphenophorus/Foto1.jpeg</t>
+    <t>Foto7.png</t>
+  </si>
+  <si>
+    <t>Foto8.png</t>
+  </si>
+  <si>
+    <t>Foto1.jpeg</t>
   </si>
 </sst>
 </file>
@@ -1573,8 +1570,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7FB08C5-DA3B-4BF7-B0CE-50F695BC8261}">
   <dimension ref="A1:AK69"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="AD58" workbookViewId="0">
-      <selection activeCell="AF73" sqref="AF73"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="AD1" workbookViewId="0">
+      <selection activeCell="AF13" sqref="AF13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1812,7 +1809,7 @@
         <v>1</v>
       </c>
       <c r="AF3" s="8" t="s">
-        <v>75</v>
+        <v>82</v>
       </c>
       <c r="AG3" s="4" t="s">
         <v>67</v>
@@ -1901,7 +1898,7 @@
         <v>2</v>
       </c>
       <c r="AF4" s="8" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="AG4" s="4" t="s">
         <v>69</v>
@@ -1990,7 +1987,7 @@
         <v>2</v>
       </c>
       <c r="AF5" s="8" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AG5" s="4" t="s">
         <v>70</v>
@@ -2079,7 +2076,7 @@
         <v>4</v>
       </c>
       <c r="AF6" s="8" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="AG6" s="4" t="s">
         <v>71</v>
@@ -2168,7 +2165,7 @@
         <v>2</v>
       </c>
       <c r="AF7" s="8" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="AG7" s="4" t="s">
         <v>72</v>
@@ -2257,7 +2254,7 @@
         <v>4</v>
       </c>
       <c r="AF8" s="8" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="AG8" s="4" t="s">
         <v>73</v>
@@ -7304,13 +7301,13 @@
       <c r="AD68" s="4"/>
       <c r="AE68" s="4"/>
       <c r="AF68" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="AG68" s="4" t="s">
         <v>67</v>
       </c>
       <c r="AH68" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="AI68" s="4" t="s">
         <v>68</v>
@@ -7384,13 +7381,13 @@
       <c r="AD69" s="4"/>
       <c r="AE69" s="4"/>
       <c r="AF69" s="4" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="AG69" s="4" t="s">
         <v>67</v>
       </c>
       <c r="AH69" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="AI69" s="4" t="s">
         <v>68</v>

</xml_diff>